<commit_message>
Limpiar mailto en plantilla
</commit_message>
<xml_diff>
--- a/assets/templates/PLANTILLA_INGRESO.xlsx
+++ b/assets/templates/PLANTILLA_INGRESO.xlsx
@@ -1213,7 +1213,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:AF974"/>
+  <dimension ref="A1:AF974"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
@@ -1382,11 +1382,7 @@
           <t>Email de facturación</t>
         </is>
       </c>
-      <c r="C13" s="22" t="inlineStr">
-        <is>
-          <t>mailto:MARCELO.VARGAS@EDALTEC.CL</t>
-        </is>
-      </c>
+      <c r="C13" s="22" t="n"/>
       <c r="E13" s="93" t="n"/>
       <c r="F13" s="92" t="n"/>
       <c r="AD13" s="1" t="n"/>
@@ -12494,9 +12490,6 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="E6:E12"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>